<commit_message>
Updated TC_27_28_29_30 Sheet test data
</commit_message>
<xml_diff>
--- a/Test Data/TC_27_28_Verify_Add_Unit_Details_For_Pro32xD_Pro32xBB_Pro16xD_Pro16xBB.xlsx
+++ b/Test Data/TC_27_28_Verify_Add_Unit_Details_For_Pro32xD_Pro32xBB_Pro16xD_Pro16xBB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CED0B7D-F837-41BC-95A8-5AE62EC2A8C5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A262921-5FAA-4DF3-8B60-1915C6ED898A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="50">
   <si>
     <t>Color Codes</t>
   </si>
@@ -931,7 +931,7 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1220,7 +1220,7 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1476,11 +1476,11 @@
       <c r="K10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="M10" s="14" t="s">
-        <v>20</v>
+      <c r="L10" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" s="14" t="b">
+        <v>0</v>
       </c>
       <c r="N10" s="14" t="s">
         <v>41</v>
@@ -1506,7 +1506,7 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1757,11 +1757,11 @@
       <c r="K10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="M10" s="14" t="s">
-        <v>20</v>
+      <c r="L10" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" s="14" t="b">
+        <v>0</v>
       </c>
       <c r="N10" s="14" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Updated slot card related test cases and test data
</commit_message>
<xml_diff>
--- a/Test Data/TC_27_28_Verify_Add_Unit_Details_For_Pro32xD_Pro32xBB_Pro16xD_Pro16xBB.xlsx
+++ b/Test Data/TC_27_28_Verify_Add_Unit_Details_For_Pro32xD_Pro32xBB_Pro16xD_Pro16xBB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A262921-5FAA-4DF3-8B60-1915C6ED898A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC9BF1D-CB11-474D-8B13-87F0D0E351B1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="51">
   <si>
     <t>Color Codes</t>
   </si>
@@ -181,10 +181,13 @@
     <t>Other Slot Cards  (2 of 4)</t>
   </si>
   <si>
-    <t>Other Slot Cards  (5 of 5)</t>
-  </si>
-  <si>
     <t>Other Slot Cards  (2 of 2)</t>
+  </si>
+  <si>
+    <t>Other Slot Cards  (3 of 18)</t>
+  </si>
+  <si>
+    <t>Other Slot Cards  (7 of 17)</t>
   </si>
 </sst>
 </file>
@@ -628,7 +631,7 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -861,7 +864,7 @@
       </c>
       <c r="R9" s="12"/>
     </row>
-    <row r="10" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
@@ -898,20 +901,20 @@
       <c r="L10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="M10" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="N10" s="14" t="s">
-        <v>15</v>
+      <c r="M10" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" s="14" t="b">
+        <v>0</v>
       </c>
       <c r="O10" s="14" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="P10" s="14" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q10" s="14" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="R10" s="14" t="s">
         <v>36</v>
@@ -930,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467CF894-130A-4F79-AEEC-497758661F02}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1176,7 +1179,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="5">
         <v>1</v>
@@ -1187,23 +1190,23 @@
       <c r="J10" s="5">
         <v>3</v>
       </c>
-      <c r="K10" s="14" t="s">
-        <v>15</v>
+      <c r="K10" s="14" t="b">
+        <v>0</v>
       </c>
       <c r="L10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="M10" s="14" t="s">
-        <v>15</v>
+      <c r="M10" s="14" t="b">
+        <v>0</v>
       </c>
       <c r="N10" s="14" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="O10" s="14" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="P10" s="14" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1220,7 +1223,7 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1483,7 +1486,7 @@
         <v>0</v>
       </c>
       <c r="N10" s="14" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="O10" s="14" t="s">
         <v>20</v>
@@ -1506,7 +1509,7 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1764,7 +1767,7 @@
         <v>0</v>
       </c>
       <c r="N10" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O10" s="14" t="s">
         <v>20</v>
@@ -2128,7 +2131,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>34</v>
       </c>
@@ -2184,7 +2187,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>25</v>
       </c>
@@ -2240,7 +2243,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>25</v>
       </c>
@@ -2296,7 +2299,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>34</v>
       </c>

</xml_diff>